<commit_message>
created BOM and CPL and removed the 10 pin JTAG/SWD in favor of just 3 pins for SWD
</commit_message>
<xml_diff>
--- a/rev2/manufacturing/BOM.xlsx
+++ b/rev2/manufacturing/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mexic\OneDrive\Documents\GitHub\PCB_practice\rev2\manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D4ED73-9488-4DB8-B357-889E9A6EB453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BF1A46-425A-4EF9-B7D1-9E4E67766215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Comment</t>
   </si>
@@ -48,15 +48,6 @@
     <t>C21,C22,C23</t>
   </si>
   <si>
-    <t>C24, C30-C33, C38-C46, C48</t>
-  </si>
-  <si>
-    <t>500n</t>
-  </si>
-  <si>
-    <t>C25</t>
-  </si>
-  <si>
     <t>9p</t>
   </si>
   <si>
@@ -118,6 +109,111 @@
   </si>
   <si>
     <t>C76617</t>
+  </si>
+  <si>
+    <t>PWR_USB</t>
+  </si>
+  <si>
+    <t>USB_OTG</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>C191124</t>
+  </si>
+  <si>
+    <t>C177673</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> R4, R5</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  J9</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    R3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    SW1</t>
+  </si>
+  <si>
+    <t>SW_Push</t>
+  </si>
+  <si>
+    <t>SPST_PTS645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    SW2</t>
+  </si>
+  <si>
+    <t>SW_SPDT</t>
+  </si>
+  <si>
+    <t>PCM12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> U2, U3</t>
+  </si>
+  <si>
+    <t>TJA1051T</t>
+  </si>
+  <si>
+    <t>SOIC-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    U4</t>
+  </si>
+  <si>
+    <t>LSM6DSOX</t>
+  </si>
+  <si>
+    <t>LGA-14</t>
+  </si>
+  <si>
+    <t>C5342108</t>
+  </si>
+  <si>
+    <t>C481766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    U5</t>
+  </si>
+  <si>
+    <t>AMS1117-3.3</t>
+  </si>
+  <si>
+    <t>SOT-223-3</t>
+  </si>
+  <si>
+    <t>C6186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    U6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Y1</t>
+  </si>
+  <si>
+    <t>16MHz</t>
+  </si>
+  <si>
+    <t>SMD_3225</t>
+  </si>
+  <si>
+    <t>C135998</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t>C24, C30-33, C38-46, C48</t>
   </si>
 </sst>
 </file>
@@ -442,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +577,7 @@
         <v>603</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -489,108 +585,238 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3">
+        <v>603</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
-        <v>603</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
       <c r="C4">
         <v>603</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
       <c r="C5">
         <v>603</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
       <c r="C6">
         <v>603</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
       <c r="C7">
         <v>603</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
       <c r="C8">
         <v>603</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="C9">
-        <v>603</v>
-      </c>
       <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>23</v>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12">
+        <v>603</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>120</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13">
+        <v>603</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>